<commit_message>
fix number to string
</commit_message>
<xml_diff>
--- a/example/input/config.xlsx
+++ b/example/input/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="configMap" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,6 +143,10 @@
   </si>
   <si>
     <t>真实年龄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -549,7 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -652,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -694,7 +698,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>

</xml_diff>